<commit_message>
Added simulations sheet for Run31
</commit_message>
<xml_diff>
--- a/config/31st/Run_Parameters_Run31.xlsx
+++ b/config/31st/Run_Parameters_Run31.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacopo\Documents\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlenardo/Research/Software/StanfordTPCAnalysis/config/31st/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96A4C00-2791-4847-B24D-B532DF761C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEA69E6-F0FA-B34F-BE4F-912C4E966F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="26980" windowHeight="15940" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20201023_DS04_BkgData_1200ADCTh" sheetId="13" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="20201103_DS25_Run220Data" sheetId="25" r:id="rId14"/>
     <sheet name="20201103_DS26_Run220Data" sheetId="26" r:id="rId15"/>
     <sheet name="20201104_DS27_Run220Data" sheetId="27" r:id="rId16"/>
+    <sheet name="simulations" sheetId="28" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="12">
   <si>
     <t>Parameter</t>
   </si>
@@ -352,12 +353,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -365,7 +366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -373,7 +374,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -381,7 +382,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -389,7 +390,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -397,7 +398,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -405,7 +406,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -413,7 +414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -421,7 +422,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -429,7 +430,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -437,7 +438,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -458,12 +459,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -479,7 +480,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -487,7 +488,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -495,7 +496,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -503,7 +504,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -511,7 +512,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -519,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -527,7 +528,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -535,7 +536,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -543,7 +544,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -564,12 +565,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -585,7 +586,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -593,7 +594,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -601,7 +602,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -609,7 +610,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -617,7 +618,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -625,7 +626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -633,7 +634,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -641,7 +642,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -649,7 +650,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -670,12 +671,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -691,7 +692,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -699,7 +700,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -707,7 +708,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -715,7 +716,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -723,7 +724,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -731,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -739,7 +740,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -747,7 +748,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -755,7 +756,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -773,15 +774,15 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,7 +790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -797,7 +798,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -805,7 +806,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -813,7 +814,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -821,7 +822,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -829,7 +830,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -837,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -845,7 +846,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -853,7 +854,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -861,7 +862,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -882,12 +883,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -903,7 +904,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -911,7 +912,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -919,7 +920,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -927,7 +928,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -935,7 +936,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -943,7 +944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -951,7 +952,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -959,7 +960,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -967,7 +968,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -988,12 +989,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +1010,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1025,7 +1026,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1041,7 +1042,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1049,7 +1050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1065,7 +1066,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1074,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1090,16 +1091,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A8FDB2-31AC-4936-8E5B-6086E9ACAA38}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1115,7 +1116,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1131,7 +1132,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1139,7 +1140,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1147,7 +1148,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1172,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1179,7 +1180,114 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDBA91A-3153-D84B-BC37-485B4428738A}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7.8125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1200,12 +1308,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1213,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1221,7 +1329,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1229,7 +1337,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1237,7 +1345,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1245,7 +1353,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1253,7 +1361,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1269,7 +1377,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1277,7 +1385,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1285,7 +1393,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1306,12 +1414,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1327,7 +1435,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1335,7 +1443,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1343,7 +1451,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1351,7 +1459,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1359,7 +1467,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1375,7 +1483,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1383,7 +1491,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1391,7 +1499,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1412,12 +1520,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1433,7 +1541,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1441,7 +1549,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1449,7 +1557,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1457,7 +1565,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1465,7 +1573,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1473,7 +1581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1481,7 +1589,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1597,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1497,7 +1605,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1518,12 +1626,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1539,7 +1647,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1547,7 +1655,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1555,7 +1663,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1563,7 +1671,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1679,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1579,7 +1687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1587,7 +1695,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1595,7 +1703,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1603,7 +1711,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1624,12 +1732,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1645,7 +1753,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1653,7 +1761,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1661,7 +1769,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1669,7 +1777,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1677,7 +1785,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1685,7 +1793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1693,7 +1801,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1701,7 +1809,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1709,7 +1817,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1730,12 +1838,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1751,7 +1859,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1759,7 +1867,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1767,7 +1875,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1775,7 +1883,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1783,7 +1891,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1791,7 +1899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1799,7 +1907,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1807,7 +1915,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1815,7 +1923,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1836,12 +1944,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1857,7 +1965,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1865,7 +1973,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1873,7 +1981,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1881,7 +1989,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1889,7 +1997,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1897,7 +2005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1905,7 +2013,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1913,7 +2021,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1921,7 +2029,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1942,12 +2050,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1963,7 +2071,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1971,7 +2079,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1979,7 +2087,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1987,7 +2095,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1995,7 +2103,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2003,7 +2111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2011,7 +2119,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2019,7 +2127,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2027,7 +2135,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Added a notebook that starts the Transverse Lifetime investigation and added some functions to the LifetimeEstimation class, the bones of which could possibly be used to carry out this investigation. Very much a work in progress and needs lots of improvement before continuation.
</commit_message>
<xml_diff>
--- a/config/31st/Run_Parameters_Run31.xlsx
+++ b/config/31st/Run_Parameters_Run31.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacopo\Documents\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brianlenardo/Research/Software/StanfordTPCAnalysis/config/31st/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96A4C00-2791-4847-B24D-B532DF761C52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AEA69E6-F0FA-B34F-BE4F-912C4E966F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" firstSheet="14" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="26980" windowHeight="15940" firstSheet="12" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20201023_DS04_BkgData_1200ADCTh" sheetId="13" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="20201103_DS25_Run220Data" sheetId="25" r:id="rId14"/>
     <sheet name="20201103_DS26_Run220Data" sheetId="26" r:id="rId15"/>
     <sheet name="20201104_DS27_Run220Data" sheetId="27" r:id="rId16"/>
+    <sheet name="simulations" sheetId="28" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="12">
   <si>
     <t>Parameter</t>
   </si>
@@ -352,12 +353,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -365,7 +366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -373,7 +374,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -381,7 +382,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -389,7 +390,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -397,7 +398,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -405,7 +406,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -413,7 +414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -421,7 +422,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -429,7 +430,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -437,7 +438,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -458,12 +459,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -471,7 +472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -479,7 +480,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -487,7 +488,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -495,7 +496,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -503,7 +504,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -511,7 +512,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -519,7 +520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -527,7 +528,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -535,7 +536,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -543,7 +544,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -564,12 +565,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -585,7 +586,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -593,7 +594,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -601,7 +602,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -609,7 +610,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -617,7 +618,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -625,7 +626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -633,7 +634,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -641,7 +642,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -649,7 +650,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -670,12 +671,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -691,7 +692,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -699,7 +700,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -707,7 +708,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -715,7 +716,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -723,7 +724,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -731,7 +732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -739,7 +740,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -747,7 +748,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -755,7 +756,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -773,15 +774,15 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,7 +790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -797,7 +798,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -805,7 +806,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -813,7 +814,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -821,7 +822,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -829,7 +830,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -837,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -845,7 +846,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -853,7 +854,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -861,7 +862,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -882,12 +883,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -903,7 +904,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -911,7 +912,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -919,7 +920,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -927,7 +928,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -935,7 +936,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -943,7 +944,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -951,7 +952,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -959,7 +960,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -967,7 +968,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -988,12 +989,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1009,7 +1010,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1017,7 +1018,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1025,7 +1026,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1033,7 +1034,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1041,7 +1042,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1049,7 +1050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1065,7 +1066,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1073,7 +1074,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1090,16 +1091,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A8FDB2-31AC-4936-8E5B-6086E9ACAA38}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1107,7 +1108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1115,7 +1116,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1131,7 +1132,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1139,7 +1140,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1147,7 +1148,7 @@
         <v>1.87</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1171,7 +1172,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1179,7 +1180,114 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DDBA91A-3153-D84B-BC37-485B4428738A}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>7.8125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>11.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1200,12 +1308,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1213,7 +1321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1221,7 +1329,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1229,7 +1337,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1237,7 +1345,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1245,7 +1353,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1253,7 +1361,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1269,7 +1377,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1277,7 +1385,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1285,7 +1393,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1306,12 +1414,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1327,7 +1435,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1335,7 +1443,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1343,7 +1451,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1351,7 +1459,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1359,7 +1467,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1367,7 +1475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1375,7 +1483,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1383,7 +1491,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1391,7 +1499,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1412,12 +1520,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1425,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1433,7 +1541,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1441,7 +1549,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1449,7 +1557,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1457,7 +1565,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1465,7 +1573,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1473,7 +1581,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1481,7 +1589,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1597,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1497,7 +1605,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1518,12 +1626,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1531,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1539,7 +1647,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1547,7 +1655,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1555,7 +1663,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1563,7 +1671,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1571,7 +1679,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1579,7 +1687,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1587,7 +1695,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1595,7 +1703,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1603,7 +1711,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1624,12 +1732,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1637,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1645,7 +1753,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1653,7 +1761,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1661,7 +1769,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1669,7 +1777,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1677,7 +1785,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1685,7 +1793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1693,7 +1801,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1701,7 +1809,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1709,7 +1817,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1730,12 +1838,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1743,7 +1851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1751,7 +1859,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1759,7 +1867,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1767,7 +1875,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1775,7 +1883,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1783,7 +1891,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1791,7 +1899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1799,7 +1907,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1807,7 +1915,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1815,7 +1923,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1836,12 +1944,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1857,7 +1965,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1865,7 +1973,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1873,7 +1981,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1881,7 +1989,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1889,7 +1997,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -1897,7 +2005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1905,7 +2013,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1913,7 +2021,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1921,7 +2029,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1942,12 +2050,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1955,7 +2063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1963,7 +2071,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1971,7 +2079,7 @@
         <v>7.8125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1979,7 +2087,7 @@
         <v>11.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1987,7 +2095,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1995,7 +2103,7 @@
         <v>1.79</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2003,7 +2111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -2011,7 +2119,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -2019,7 +2127,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -2027,7 +2135,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>

</xml_diff>